<commit_message>
changes in accelerometer to haptuator program | two haptuator functionality support
</commit_message>
<xml_diff>
--- a/Accelerometer and Audio data/IMU and ADXL data/Excel data and plotting program/Gravel Road_adxl-3200Hz-16g_imu-562Hz-16g.xlsx
+++ b/Accelerometer and Audio data/IMU and ADXL data/Excel data and plotting program/Gravel Road_adxl-3200Hz-16g_imu-562Hz-16g.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GEM Lab\GEMLabHCIResearch\Accelerometer and Audio data\IMU and ADXL data\Excel data and plotting program\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C18314D3-2CBD-4494-83D4-F4AB59FC3E37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EABA1688-F9F4-4A31-8687-34DB8CA03529}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -46,9 +46,6 @@
     <t>IMU-Z</t>
   </si>
   <si>
-    <t xml:space="preserve"> ADXL-X</t>
-  </si>
-  <si>
     <t>ADXL-Y</t>
   </si>
   <si>
@@ -62,6 +59,9 @@
   </si>
   <si>
     <t>ADXL Magnitude</t>
+  </si>
+  <si>
+    <t>ADXL-X</t>
   </si>
 </sst>
 </file>
@@ -904,15 +904,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{581A2E54-B9F6-411E-85D9-77D789881CE3}">
   <dimension ref="A1:J181"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A144" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2:J181"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -924,19 +924,19 @@
         <v>2</v>
       </c>
       <c r="E1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H1" t="s">
+        <v>3</v>
+      </c>
+      <c r="I1" t="s">
+        <v>4</v>
+      </c>
+      <c r="J1" t="s">
         <v>7</v>
-      </c>
-      <c r="G1" t="s">
-        <v>3</v>
-      </c>
-      <c r="H1" t="s">
-        <v>4</v>
-      </c>
-      <c r="I1" t="s">
-        <v>5</v>
-      </c>
-      <c r="J1" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
@@ -6528,15 +6528,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73D2FF61-A8E6-4236-9040-00E84C873F41}">
   <dimension ref="A1:J200"/>
   <sheetViews>
-    <sheetView topLeftCell="A162" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="M194" sqref="M194"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -6548,19 +6548,19 @@
         <v>2</v>
       </c>
       <c r="E1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H1" t="s">
+        <v>3</v>
+      </c>
+      <c r="I1" t="s">
+        <v>4</v>
+      </c>
+      <c r="J1" t="s">
         <v>7</v>
-      </c>
-      <c r="G1" t="s">
-        <v>3</v>
-      </c>
-      <c r="H1" t="s">
-        <v>4</v>
-      </c>
-      <c r="I1" t="s">
-        <v>5</v>
-      </c>
-      <c r="J1" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
@@ -12741,15 +12741,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J199"/>
   <sheetViews>
-    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2:J199"/>
+    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -12761,19 +12761,19 @@
         <v>2</v>
       </c>
       <c r="E1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H1" t="s">
+        <v>3</v>
+      </c>
+      <c r="I1" t="s">
+        <v>4</v>
+      </c>
+      <c r="J1" t="s">
         <v>7</v>
-      </c>
-      <c r="G1" t="s">
-        <v>3</v>
-      </c>
-      <c r="H1" t="s">
-        <v>4</v>
-      </c>
-      <c r="I1" t="s">
-        <v>5</v>
-      </c>
-      <c r="J1" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">

</xml_diff>